<commit_message>
latest updates, from Liz/DWG work
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="442" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="1058">
   <si>
     <t>table</t>
   </si>
@@ -2510,7 +2510,19 @@
     <t>antibody</t>
   </si>
   <si>
-    <t>2012-10-12</t>
+    <t>AR:4</t>
+  </si>
+  <si>
+    <t>AR_Center_ID</t>
+  </si>
+  <si>
+    <t>Antibody HMS LINCS ID</t>
+  </si>
+  <si>
+    <t>HMS LINCS ID</t>
+  </si>
+  <si>
+    <t>HMS LINCS-specific antibody ID</t>
   </si>
   <si>
     <t>AR:1</t>
@@ -2522,19 +2534,7 @@
     <t>Antibody Name</t>
   </si>
   <si>
-    <t>The primary name of the antibody as chosen by LINCS</t>
-  </si>
-  <si>
-    <t>AR:2</t>
-  </si>
-  <si>
-    <t>AR_ID</t>
-  </si>
-  <si>
-    <t>Antibody LINCS ID</t>
-  </si>
-  <si>
-    <t>Unique identifier of antibody reagent</t>
+    <t>Antibody name according to the vendor or provider</t>
   </si>
   <si>
     <t>AR:3</t>
@@ -2543,19 +2543,61 @@
     <t>AR_Alternative_Name</t>
   </si>
   <si>
-    <t>List of synonymous antibody names, including the primary name</t>
-  </si>
-  <si>
-    <t>AR:4</t>
-  </si>
-  <si>
-    <t>AR_Center_ID</t>
-  </si>
-  <si>
-    <t>Ab HMS LINCS ID</t>
-  </si>
-  <si>
-    <t>Center specific ID for antibody</t>
+    <t>Alternative Names</t>
+  </si>
+  <si>
+    <t>Other names for the antibody</t>
+  </si>
+  <si>
+    <t>Other names for the antibody. If no synonyms are provided, leave blank.</t>
+  </si>
+  <si>
+    <t>clone_name</t>
+  </si>
+  <si>
+    <t>AR:new1</t>
+  </si>
+  <si>
+    <t>AR_Clone_Name</t>
+  </si>
+  <si>
+    <t>Clone Name</t>
+  </si>
+  <si>
+    <t>Monoclonal clone name/ID #</t>
+  </si>
+  <si>
+    <t>Monoclonal clone name/ID #. If not relevant, leave blank.</t>
+  </si>
+  <si>
+    <t>antibody_registry_id</t>
+  </si>
+  <si>
+    <t>AR:2mod</t>
+  </si>
+  <si>
+    <t>AR_RRID</t>
+  </si>
+  <si>
+    <t>Resource Identification Initiative ID</t>
+  </si>
+  <si>
+    <t>Antibody RRID according to Antibody Registry</t>
+  </si>
+  <si>
+    <t>Resource Identification Initiative ID (RRID) from Antibody Registry. If the antibody is not yet registered in Antibody Registry, the user should register it him/herself or ask the vendor to register it.</t>
+  </si>
+  <si>
+    <t>AR:new2</t>
+  </si>
+  <si>
+    <t>AR_LINCS_ID</t>
+  </si>
+  <si>
+    <t>Global LINCS ID</t>
+  </si>
+  <si>
+    <t>Global LINCS antibody ID</t>
   </si>
   <si>
     <t>target_protein_name</t>
@@ -2567,7 +2609,13 @@
     <t>AR_Target_Protein</t>
   </si>
   <si>
-    <t>The name of the protein (target), which is the recommended name from the UniProt database. If the name of a related entity is used instead, this should be documented explicitly in AR_Immunogen.</t>
+    <t>Protein Target of Antibody</t>
+  </si>
+  <si>
+    <t>Nominal protein target, based on the recommended name from UniProt. If the target is not a protein ("N/A"), see information below.</t>
+  </si>
+  <si>
+    <t>Nominal protein target, based on the recommended name from UniProt. If the name of a related entity is used instead, this should be documented explicitly in AR_Immunogen. If the target is not a protein, enter "N/A" and complete the "non-protein target" row below.</t>
   </si>
   <si>
     <t>target_protein_uniprot_id</t>
@@ -2579,28 +2627,67 @@
     <t>AR_Target_Protein_ID</t>
   </si>
   <si>
-    <t>The UniProt ID of the protein targeted by the antibody, if available. If the UniProt ID of a related entity is used instead, this should be documented explicitly.</t>
-  </si>
-  <si>
-    <t>target_gene_name</t>
-  </si>
-  <si>
-    <t>AR:10</t>
-  </si>
-  <si>
-    <t>AR_Target_Gene</t>
-  </si>
-  <si>
-    <t>The NCBI gene name. In cases where the protein is modified (the protein sequence differs from the sequence encoded by the gene listed), it should be described in AR_Immunogen.</t>
-  </si>
-  <si>
-    <t>target_gene_id</t>
-  </si>
-  <si>
-    <t>AR:11</t>
-  </si>
-  <si>
-    <t>AR_Target_Gene ID</t>
+    <t>Protein Target UniProt ID</t>
+  </si>
+  <si>
+    <t>UniProt ID of the nominal protein target of the antibody. If the target is not a protein ("N/A"), see information below.</t>
+  </si>
+  <si>
+    <t>UniProt ID of the nominal protein target of the antibody. If the UniProt ID of a related entity is used instead, this should be documented explicitly in AR_Immunogen. If the target is not a protein, enter "N/A" and complete the "non-protein target" row below. [for display on protein registration page, not antibody registration page]</t>
+  </si>
+  <si>
+    <t>target_protein_facility_id</t>
+  </si>
+  <si>
+    <t>AR:new3</t>
+  </si>
+  <si>
+    <t>AR_Target_Protein_Center_ID</t>
+  </si>
+  <si>
+    <t>Protein Target HMS LINCS ID</t>
+  </si>
+  <si>
+    <t>Protein target HMS LINCS ID</t>
+  </si>
+  <si>
+    <t>HMS LINCS-specific protein ID for the antibody target protein</t>
+  </si>
+  <si>
+    <t>target_protein_lincs_id</t>
+  </si>
+  <si>
+    <t>AR:new4</t>
+  </si>
+  <si>
+    <t>AR_Target_Protein_LINCS_ID</t>
+  </si>
+  <si>
+    <t>Protein Target LINCS ID</t>
+  </si>
+  <si>
+    <t>Protein target global LINCS ID</t>
+  </si>
+  <si>
+    <t>Global LINCS-specific protein ID for the antibody target protein [for display on protein registration page, not antibody registration page]</t>
+  </si>
+  <si>
+    <t>non_protein_target_name</t>
+  </si>
+  <si>
+    <t>AR:new5</t>
+  </si>
+  <si>
+    <t>AR_Non-Protein_Target</t>
+  </si>
+  <si>
+    <t>Non-protein Target of Antibody</t>
+  </si>
+  <si>
+    <t>Nominal target if not a protein. If the target is a protein ("N/A"), see information above.</t>
+  </si>
+  <si>
+    <t>Name of the nominal target of the antibody if not a protein. Use common English vocabulary. You can quote the vendor catalog or provider. If the target is a protein, complete the rows above instead and enter "N/A" in this row.</t>
   </si>
   <si>
     <t>target_organism</t>
@@ -2612,7 +2699,31 @@
     <t>AR_Target_Organism</t>
   </si>
   <si>
-    <t>The organism of the target protein/gene described in AR:7-AR:10; NCBI nomenclature (e.g. Homo sapiens).</t>
+    <t>Organism of Target of Antibody</t>
+  </si>
+  <si>
+    <t>Organism of target</t>
+  </si>
+  <si>
+    <t>Organism of the target protein. Use standardized NCBI Taxon nomenclature (e.g. Homo sapiens).</t>
+  </si>
+  <si>
+    <t>antibody_type</t>
+  </si>
+  <si>
+    <t>AR:new6</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Type</t>
+  </si>
+  <si>
+    <t>Antibody Type</t>
+  </si>
+  <si>
+    <t>Specification of antibody as natural or engineered</t>
+  </si>
+  <si>
+    <t>Specification of antibody as "natural" (immunologically selected in an animal) or "engineered"</t>
   </si>
   <si>
     <t>immunogen</t>
@@ -2624,7 +2735,13 @@
     <t>AR_Immunogen</t>
   </si>
   <si>
-    <t>A complete description of the immunogen used to make the antibody (text). This description should include the source of the immunogen (e.g. recombinantly expressed in E. coli, purified from canine pancreas, etc.). Any references relevant to the immunogen or making of the antibody can be listed in AR_Relevant_Reference.</t>
+    <t>Immunogen / Epitope Selection Entity</t>
+  </si>
+  <si>
+    <t>Complete description of immunogen or entity used to select epitope</t>
+  </si>
+  <si>
+    <t>Complete description of the immunogen (if produced in an animal) or entity used to select the epitope (if selected in vitro), including the source of the immunogen/entity (e.g. recombinantly expressed in E. coli, purified from canine pancreas) and its method of preparation. Any references relevant to the immunogen/target or production of the antibody should be listed in AR_Relevant_Reference. You can quote the vendor and cite it as the source.</t>
   </si>
   <si>
     <t>immunogen_sequence</t>
@@ -2636,31 +2753,67 @@
     <t>AR_Immunogen_Sequence</t>
   </si>
   <si>
-    <t>If the immunogen is a peptide, protein fragment, or small protein, the amino acid sequence should be provided.</t>
-  </si>
-  <si>
-    <t>antibody_clonality</t>
+    <t>Immunogen Sequence</t>
+  </si>
+  <si>
+    <t>Sequence of immunogen or entity used to select epitope</t>
+  </si>
+  <si>
+    <t>Complete amino acid sequence of the immunogen or entity used to select the epitope if it was a peptide, protein fragment, or small protein. If not provided, leave blank.</t>
+  </si>
+  <si>
+    <t>AR:16mod</t>
+  </si>
+  <si>
+    <t>AR_Source_Organism</t>
+  </si>
+  <si>
+    <t>Source Organism for Antibody Production</t>
+  </si>
+  <si>
+    <t>Source organism for antibody production</t>
+  </si>
+  <si>
+    <t>Organism or cell type used to produce the antibody. Use common English names (e.g. mouse, rabbit, horse, baculovirus cells).</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>AR:new7</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Species</t>
+  </si>
+  <si>
+    <t>Antibody Fc Domain Source Species</t>
+  </si>
+  <si>
+    <t>Antibody Fc domain source species</t>
+  </si>
+  <si>
+    <t>Organism from which the antibody was derived if produced in an animal or  species from which the Fc domain of the antibody was derived if the antibody was engineered</t>
+  </si>
+  <si>
+    <t>clonality</t>
   </si>
   <si>
     <t>AR:15</t>
   </si>
   <si>
-    <t>AR_AntibodyClonality</t>
-  </si>
-  <si>
-    <t>A controlled vocabulary specifying whether the antibody is polyclonal or monoclonal.</t>
-  </si>
-  <si>
-    <t>AR:16</t>
-  </si>
-  <si>
-    <t>AR_Source_Organism</t>
-  </si>
-  <si>
-    <t>A controlled vocabulary describing the source of the antibody (e.g. mouse, rabbit, horse, goat, etc.)</t>
-  </si>
-  <si>
-    <t>antibody_isotype</t>
+    <t>AR_Antibody_Clonality</t>
+  </si>
+  <si>
+    <t>Antibody Clonality</t>
+  </si>
+  <si>
+    <t>Mono- or polyclonality of antibody</t>
+  </si>
+  <si>
+    <t>Identification of the antibody as monoclonal or polyclonal</t>
+  </si>
+  <si>
+    <t>isotype</t>
   </si>
   <si>
     <t>AR:17</t>
@@ -2669,22 +2822,151 @@
     <t>AR_Antibody_Isotype</t>
   </si>
   <si>
-    <t>A controlled vocabulary describing the antibody isotype (e.g. IgG, IgM, etc.)</t>
-  </si>
-  <si>
-    <t>engineering</t>
+    <t>Antibody Isotype</t>
+  </si>
+  <si>
+    <t>Isotype of antibody Fc domain</t>
+  </si>
+  <si>
+    <t>Isotype (e.g. IgG2,IgM, etc.) of the Fc domain of the antibody or antibody mixture if polyclonal</t>
+  </si>
+  <si>
+    <t>production_details</t>
   </si>
   <si>
     <t>AR:18</t>
   </si>
   <si>
-    <t>AR_Engineering</t>
-  </si>
-  <si>
-    <t>Is the antibody engineered/produced in an animal? Yes/No. If yes, then information should be provided about the engineering method and the production method (produced in mammalian cells, insect cells, yeast, bacteria, etc.).</t>
-  </si>
-  <si>
-    <t>antibody_purity</t>
+    <t>AR_Antibody_Production_Details</t>
+  </si>
+  <si>
+    <t>Antibody Production Details</t>
+  </si>
+  <si>
+    <t>Antibody production details</t>
+  </si>
+  <si>
+    <t>If the antibody was produced originally in an animal, including if it is currently derived from hybridoma cells, this field includes relevant information about the antibody production method that is not captured in other fields. If the antibody was engineered, this field includes information about the methods used to engineer and produce the antibody (e.g. humanized mouse antibody sequence expressed in and protein A-purified from yeast cells) and any other relevant details not captured in other fields. Any references relevant to antibody production should be listed in AR_Relevant_References.</t>
+  </si>
+  <si>
+    <t>labeling</t>
+  </si>
+  <si>
+    <t>AR:20</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Labeling</t>
+  </si>
+  <si>
+    <t>Antibody Conjugation or Labeling</t>
+  </si>
+  <si>
+    <t>Antibody conjugation or labeling</t>
+  </si>
+  <si>
+    <t>If the antibody was labeled or conjugated, what fluor or enzyme (e.g. horseradish peroxidase) was conjugated to the antibody.</t>
+  </si>
+  <si>
+    <t>labeling_details</t>
+  </si>
+  <si>
+    <t>AR:new8</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Labeling_Details</t>
+  </si>
+  <si>
+    <t>Antibody Conjugation or Labeling Information</t>
+  </si>
+  <si>
+    <t>Antibody conjugation or labeling details</t>
+  </si>
+  <si>
+    <t>If the antibody was labeled or conjugated, this field includes information about the protocol used to conjugate the fluor or enzyme to the antibody. Any references relevant to antibody labeling should be listed in AR_Relevant_References.</t>
+  </si>
+  <si>
+    <t>relevant_references</t>
+  </si>
+  <si>
+    <t>AR:22</t>
+  </si>
+  <si>
+    <t>AR_Relevant_References</t>
+  </si>
+  <si>
+    <t>Relevant References</t>
+  </si>
+  <si>
+    <t>Relevant references</t>
+  </si>
+  <si>
+    <t>Relevant literature references for antibody generation or labeling as PMIDs or patent numbers</t>
+  </si>
+  <si>
+    <t>antibodybatch</t>
+  </si>
+  <si>
+    <t>ARB:HMS_BATCH_ID</t>
+  </si>
+  <si>
+    <t>AR_Batch_ID</t>
+  </si>
+  <si>
+    <t>HMS LINCS batch ID</t>
+  </si>
+  <si>
+    <t>Batch ID number assigned by the HMS LINCS Center</t>
+  </si>
+  <si>
+    <t>Batch ID number assigned by the HMS LINCS Center after local registration of the antibody</t>
+  </si>
+  <si>
+    <t>AR:5</t>
+  </si>
+  <si>
+    <t>AR_Provider</t>
+  </si>
+  <si>
+    <t>Antibody vendor or provider</t>
+  </si>
+  <si>
+    <t>Vendor or lab that supplied the antibody</t>
+  </si>
+  <si>
+    <t>Vendor or lab that supplied the antibody. Use standardized vendor/provider names.</t>
+  </si>
+  <si>
+    <t>AR:6</t>
+  </si>
+  <si>
+    <t>AR_Provider_Catalog_ ID</t>
+  </si>
+  <si>
+    <t>Antibody vendor catalog number or provider ID </t>
+  </si>
+  <si>
+    <t>ID or catalog number(s) assigned by the vendor or provider</t>
+  </si>
+  <si>
+    <t>ID or catalog number(s) assigned to the antibody by the vendor or provider and associated with the listed Antibody Registry RRID. Due to degeneracy in Antibody Registry, more than one catalog number (e.g. for different aliquot sizes) may need to be listed.</t>
+  </si>
+  <si>
+    <t>provider_batch_id</t>
+  </si>
+  <si>
+    <t>AR:7</t>
+  </si>
+  <si>
+    <t>AR_Provider_Batch_ID</t>
+  </si>
+  <si>
+    <t>Antibody batch / lot number</t>
+  </si>
+  <si>
+    <t>Batch or lot number assigned by the vendor or provider</t>
+  </si>
+  <si>
+    <t>Batch or lot number assigned to the antibody by the vendor or provider</t>
   </si>
   <si>
     <t>AR:19</t>
@@ -2693,82 +2975,10 @@
     <t>AR_Antibody_Purity</t>
   </si>
   <si>
-    <t>A description of the antibody's level of purity (e.g., if it was purified, affinity purified, etc.)--a controlled vocabulary should be developed.</t>
-  </si>
-  <si>
-    <t>antibody_labeling</t>
-  </si>
-  <si>
-    <t>AR:20</t>
-  </si>
-  <si>
-    <t>AR_Antibody_Labeling</t>
-  </si>
-  <si>
-    <t>It should be indicated (Yes/No) whether the antibody is labeled or conjugated; If yes, with what fluor or enzyme (horseradish peroxidase)</t>
-  </si>
-  <si>
-    <t>recommended_experiment_type</t>
-  </si>
-  <si>
-    <t>AR:21</t>
-  </si>
-  <si>
-    <t>AR_Recommended_Experiment_Type</t>
-  </si>
-  <si>
-    <t>The type of experiment in which the antibody is useful, e.g., western blot, ELISA, immunostaining, etc. This depends on the ability of the antibody to recognize the native (non-denatured) or denatured target protein.</t>
-  </si>
-  <si>
-    <t>relevant_reference</t>
-  </si>
-  <si>
-    <t>AR:22</t>
-  </si>
-  <si>
-    <t>AR_Relevant_Reference</t>
-  </si>
-  <si>
-    <t>specificity</t>
-  </si>
-  <si>
-    <t>AR:23</t>
-  </si>
-  <si>
-    <t>AR_Specificity</t>
-  </si>
-  <si>
-    <t>Proteins other than the intended target with which the antibody cross-reacts. This includes homologues of the target protein from other organisms (text field; appropriate references should be provided if available).</t>
-  </si>
-  <si>
-    <t>antibodybatch</t>
-  </si>
-  <si>
-    <t>AR:5</t>
-  </si>
-  <si>
-    <t>AR_Provider</t>
-  </si>
-  <si>
-    <t>Vendor or lab that supplied the antibody</t>
-  </si>
-  <si>
-    <t>AR:6</t>
-  </si>
-  <si>
-    <t>AR_Provider_Catalog_ ID</t>
-  </si>
-  <si>
-    <t>ID or catalogue number assigned to the antibody by the vendor or provider</t>
-  </si>
-  <si>
-    <t>AR:7</t>
-  </si>
-  <si>
-    <t>AR_Batch_ID</t>
-  </si>
-  <si>
-    <t>Batch or lot number assigned to the antibody by the vendor or provider</t>
+    <t>Antibody purity</t>
+  </si>
+  <si>
+    <t>Purity of the antibody (e.g. purified, affinity purified). If not purified, enter "not purified". If unknown, enter "unknown".</t>
   </si>
   <si>
     <t>otherreagent</t>
@@ -2796,9 +3006,6 @@
   </si>
   <si>
     <t>Reagent HMS LINCS ID</t>
-  </si>
-  <si>
-    <t>HMS LINCS ID</t>
   </si>
   <si>
     <t>OR:5</t>
@@ -3055,12 +3262,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -3089,7 +3303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3122,6 +3336,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -3139,14 +3361,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR224"/>
+  <dimension ref="A1:AR229"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N200" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J178" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A200" activeCellId="0" sqref="A200"/>
-      <selection pane="bottomRight" activeCell="Q219" activeCellId="0" sqref="Q219"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A178" activeCellId="0" sqref="A178"/>
+      <selection pane="bottomRight" activeCell="O200" activeCellId="0" sqref="O200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -12509,7 +12731,7 @@
         <v>827</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="E178" s="0" t="s">
         <v>24</v>
@@ -12526,22 +12748,22 @@
       <c r="J178" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K178" s="0" t="s">
+      <c r="L178" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M178" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="L178" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M178" s="5" t="s">
+      <c r="N178" s="5" t="s">
         <v>829</v>
       </c>
-      <c r="N178" s="5" t="s">
+      <c r="O178" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="O178" s="0" t="s">
+      <c r="Q178" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="Q178" s="5" t="s">
+      <c r="S178" s="0" t="s">
         <v>832</v>
       </c>
     </row>
@@ -12550,7 +12772,7 @@
         <v>827</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>315</v>
+        <v>150</v>
       </c>
       <c r="E179" s="0" t="s">
         <v>24</v>
@@ -12567,9 +12789,6 @@
       <c r="J179" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K179" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L179" s="0" t="s">
         <v>24</v>
       </c>
@@ -12583,6 +12802,9 @@
         <v>835</v>
       </c>
       <c r="Q179" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="S179" s="0" t="s">
         <v>836</v>
       </c>
     </row>
@@ -12608,9 +12830,6 @@
       <c r="J180" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K180" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L180" s="0" t="s">
         <v>24</v>
       </c>
@@ -12620,8 +12839,14 @@
       <c r="N180" s="5" t="s">
         <v>838</v>
       </c>
+      <c r="O180" s="0" t="s">
+        <v>839</v>
+      </c>
       <c r="Q180" s="5" t="s">
-        <v>839</v>
+        <v>840</v>
+      </c>
+      <c r="S180" s="0" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12629,7 +12854,7 @@
         <v>827</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>107</v>
+        <v>842</v>
       </c>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -12648,31 +12873,31 @@
       <c r="J181" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K181" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L181" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M181" s="5" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="N181" s="5" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="O181" s="0" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="Q181" s="5" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>846</v>
+      </c>
+      <c r="S181" s="0" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>827</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -12691,20 +12916,23 @@
       <c r="J182" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K182" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L182" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M182" s="5" t="s">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="N182" s="5" t="s">
-        <v>846</v>
+        <v>850</v>
+      </c>
+      <c r="O182" s="0" t="s">
+        <v>851</v>
       </c>
       <c r="Q182" s="5" t="s">
-        <v>847</v>
+        <v>852</v>
+      </c>
+      <c r="S182" s="8" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12712,7 +12940,7 @@
         <v>827</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>848</v>
+        <v>315</v>
       </c>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -12731,36 +12959,38 @@
       <c r="J183" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K183" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L183" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M183" s="5" t="s">
-        <v>849</v>
+        <v>854</v>
       </c>
       <c r="N183" s="5" t="s">
-        <v>850</v>
+        <v>855</v>
+      </c>
+      <c r="O183" s="0" t="s">
+        <v>653</v>
       </c>
       <c r="Q183" s="5" t="s">
-        <v>851</v>
+        <v>856</v>
+      </c>
+      <c r="S183" s="0" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+      <c r="B184" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="B184" s="0" t="s">
-        <v>852</v>
-      </c>
-      <c r="C184" s="5"/>
-      <c r="D184" s="5"/>
       <c r="E184" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F184" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H184" s="0" t="s">
         <v>24</v>
@@ -12769,38 +12999,40 @@
         <v>49</v>
       </c>
       <c r="J184" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K184" s="0" t="s">
-        <v>828</v>
+        <v>25</v>
       </c>
       <c r="L184" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M184" s="5" t="s">
-        <v>853</v>
-      </c>
-      <c r="N184" s="5" t="s">
-        <v>854</v>
+        <v>859</v>
+      </c>
+      <c r="N184" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="O184" s="0" t="s">
+        <v>861</v>
       </c>
       <c r="Q184" s="5" t="s">
-        <v>855</v>
+        <v>862</v>
+      </c>
+      <c r="S184" s="0" t="s">
+        <v>863</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+      <c r="B185" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="C185" s="5"/>
+      <c r="D185" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="B185" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="C185" s="5"/>
-      <c r="D185" s="5"/>
       <c r="E185" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F185" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H185" s="0" t="s">
         <v>24</v>
@@ -12809,38 +13041,39 @@
         <v>52</v>
       </c>
       <c r="J185" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K185" s="0" t="s">
-        <v>828</v>
+        <v>25</v>
       </c>
       <c r="L185" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M185" s="5" t="s">
-        <v>857</v>
+        <v>865</v>
       </c>
       <c r="N185" s="5" t="s">
-        <v>858</v>
+        <v>866</v>
+      </c>
+      <c r="O185" s="0" t="s">
+        <v>867</v>
       </c>
       <c r="Q185" s="5" t="s">
-        <v>557</v>
+        <v>868</v>
+      </c>
+      <c r="S185" s="0" t="s">
+        <v>869</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+      <c r="B186" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="D186" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="B186" s="0" t="s">
-        <v>859</v>
-      </c>
-      <c r="C186" s="5"/>
-      <c r="D186" s="5"/>
       <c r="E186" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F186" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H186" s="0" t="s">
         <v>24</v>
@@ -12849,38 +13082,39 @@
         <v>56</v>
       </c>
       <c r="J186" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K186" s="0" t="s">
-        <v>828</v>
+        <v>25</v>
       </c>
       <c r="L186" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M186" s="5" t="s">
-        <v>860</v>
-      </c>
-      <c r="N186" s="5" t="s">
-        <v>861</v>
+      <c r="M186" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="N186" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="O186" s="0" t="s">
+        <v>873</v>
       </c>
       <c r="Q186" s="5" t="s">
-        <v>862</v>
+        <v>874</v>
+      </c>
+      <c r="S186" s="0" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
+      <c r="B187" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="D187" s="0" t="s">
         <v>827</v>
       </c>
-      <c r="B187" s="0" t="s">
-        <v>863</v>
-      </c>
-      <c r="C187" s="5"/>
-      <c r="D187" s="5"/>
       <c r="E187" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F187" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H187" s="0" t="s">
         <v>24</v>
@@ -12889,22 +13123,25 @@
         <v>59</v>
       </c>
       <c r="J187" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K187" s="0" t="s">
-        <v>828</v>
+        <v>25</v>
       </c>
       <c r="L187" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M187" s="5" t="s">
-        <v>864</v>
-      </c>
-      <c r="N187" s="5" t="s">
-        <v>865</v>
+      <c r="M187" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="N187" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="O187" s="0" t="s">
+        <v>879</v>
       </c>
       <c r="Q187" s="5" t="s">
-        <v>866</v>
+        <v>880</v>
+      </c>
+      <c r="S187" s="0" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12912,13 +13149,16 @@
         <v>827</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>867</v>
+        <v>882</v>
       </c>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
       <c r="E188" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F188" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H188" s="0" t="s">
         <v>24</v>
       </c>
@@ -12928,20 +13168,23 @@
       <c r="J188" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K188" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L188" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M188" s="5" t="s">
-        <v>868</v>
+        <v>883</v>
       </c>
       <c r="N188" s="5" t="s">
-        <v>869</v>
+        <v>884</v>
+      </c>
+      <c r="O188" s="0" t="s">
+        <v>885</v>
       </c>
       <c r="Q188" s="5" t="s">
-        <v>870</v>
+        <v>886</v>
+      </c>
+      <c r="S188" s="0" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12949,7 +13192,7 @@
         <v>827</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>871</v>
+        <v>888</v>
       </c>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -12957,7 +13200,7 @@
         <v>24</v>
       </c>
       <c r="F189" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H189" s="0" t="s">
         <v>24</v>
@@ -12968,20 +13211,23 @@
       <c r="J189" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K189" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L189" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M189" s="5" t="s">
-        <v>872</v>
+        <v>889</v>
       </c>
       <c r="N189" s="5" t="s">
-        <v>873</v>
+        <v>890</v>
+      </c>
+      <c r="O189" s="0" t="s">
+        <v>891</v>
       </c>
       <c r="Q189" s="5" t="s">
-        <v>874</v>
+        <v>892</v>
+      </c>
+      <c r="S189" s="0" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12989,7 +13235,7 @@
         <v>827</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>612</v>
+        <v>894</v>
       </c>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -12997,7 +13243,7 @@
         <v>24</v>
       </c>
       <c r="F190" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H190" s="0" t="s">
         <v>24</v>
@@ -13008,20 +13254,23 @@
       <c r="J190" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K190" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L190" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M190" s="5" t="s">
-        <v>875</v>
+        <v>895</v>
       </c>
       <c r="N190" s="5" t="s">
-        <v>876</v>
+        <v>896</v>
+      </c>
+      <c r="O190" s="0" t="s">
+        <v>897</v>
       </c>
       <c r="Q190" s="5" t="s">
-        <v>877</v>
+        <v>898</v>
+      </c>
+      <c r="S190" s="0" t="s">
+        <v>899</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13029,7 +13278,7 @@
         <v>827</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>878</v>
+        <v>900</v>
       </c>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -13037,7 +13286,7 @@
         <v>24</v>
       </c>
       <c r="F191" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H191" s="0" t="s">
         <v>24</v>
@@ -13048,20 +13297,23 @@
       <c r="J191" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K191" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L191" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M191" s="5" t="s">
-        <v>879</v>
+        <v>901</v>
       </c>
       <c r="N191" s="5" t="s">
-        <v>880</v>
+        <v>902</v>
+      </c>
+      <c r="O191" s="0" t="s">
+        <v>903</v>
       </c>
       <c r="Q191" s="5" t="s">
-        <v>881</v>
+        <v>904</v>
+      </c>
+      <c r="S191" s="0" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13069,13 +13321,16 @@
         <v>827</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>882</v>
+        <v>906</v>
       </c>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
       <c r="E192" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F192" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H192" s="0" t="s">
         <v>24</v>
       </c>
@@ -13085,20 +13340,23 @@
       <c r="J192" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K192" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L192" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M192" s="5" t="s">
-        <v>883</v>
+        <v>907</v>
       </c>
       <c r="N192" s="5" t="s">
-        <v>884</v>
+        <v>908</v>
+      </c>
+      <c r="O192" s="0" t="s">
+        <v>909</v>
       </c>
       <c r="Q192" s="5" t="s">
-        <v>885</v>
+        <v>910</v>
+      </c>
+      <c r="S192" s="0" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13106,13 +13364,16 @@
         <v>827</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>886</v>
+        <v>612</v>
       </c>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
       <c r="E193" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F193" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H193" s="0" t="s">
         <v>24</v>
       </c>
@@ -13122,20 +13383,23 @@
       <c r="J193" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K193" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L193" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M193" s="5" t="s">
-        <v>887</v>
+        <v>912</v>
       </c>
       <c r="N193" s="5" t="s">
-        <v>888</v>
+        <v>913</v>
+      </c>
+      <c r="O193" s="0" t="s">
+        <v>914</v>
       </c>
       <c r="Q193" s="5" t="s">
-        <v>889</v>
+        <v>915</v>
+      </c>
+      <c r="S193" s="0" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13143,13 +13407,16 @@
         <v>827</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>890</v>
+        <v>917</v>
       </c>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
       <c r="E194" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F194" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H194" s="0" t="s">
         <v>24</v>
       </c>
@@ -13159,20 +13426,23 @@
       <c r="J194" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K194" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L194" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M194" s="5" t="s">
-        <v>891</v>
+        <v>918</v>
       </c>
       <c r="N194" s="5" t="s">
-        <v>892</v>
+        <v>919</v>
+      </c>
+      <c r="O194" s="0" t="s">
+        <v>920</v>
       </c>
       <c r="Q194" s="5" t="s">
-        <v>893</v>
+        <v>921</v>
+      </c>
+      <c r="S194" s="0" t="s">
+        <v>922</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13180,13 +13450,16 @@
         <v>827</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>894</v>
+        <v>923</v>
       </c>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
       <c r="E195" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F195" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H195" s="0" t="s">
         <v>24</v>
       </c>
@@ -13196,20 +13469,23 @@
       <c r="J195" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K195" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L195" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M195" s="5" t="s">
-        <v>895</v>
+        <v>924</v>
       </c>
       <c r="N195" s="5" t="s">
-        <v>896</v>
+        <v>925</v>
+      </c>
+      <c r="O195" s="0" t="s">
+        <v>926</v>
       </c>
       <c r="Q195" s="5" t="s">
-        <v>897</v>
+        <v>927</v>
+      </c>
+      <c r="S195" s="0" t="s">
+        <v>928</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13217,13 +13493,16 @@
         <v>827</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>898</v>
+        <v>929</v>
       </c>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
       <c r="E196" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F196" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H196" s="0" t="s">
         <v>24</v>
       </c>
@@ -13233,20 +13512,23 @@
       <c r="J196" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K196" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L196" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M196" s="5" t="s">
-        <v>899</v>
+        <v>930</v>
       </c>
       <c r="N196" s="5" t="s">
-        <v>900</v>
+        <v>931</v>
+      </c>
+      <c r="O196" s="0" t="s">
+        <v>932</v>
       </c>
       <c r="Q196" s="5" t="s">
-        <v>622</v>
+        <v>933</v>
+      </c>
+      <c r="S196" s="0" t="s">
+        <v>934</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13254,7 +13536,7 @@
         <v>827</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>901</v>
+        <v>935</v>
       </c>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -13262,7 +13544,7 @@
         <v>24</v>
       </c>
       <c r="F197" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H197" s="0" t="s">
         <v>24</v>
@@ -13273,34 +13555,40 @@
       <c r="J197" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K197" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L197" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M197" s="5" t="s">
-        <v>902</v>
+        <v>936</v>
       </c>
       <c r="N197" s="5" t="s">
-        <v>903</v>
+        <v>937</v>
+      </c>
+      <c r="O197" s="0" t="s">
+        <v>938</v>
       </c>
       <c r="Q197" s="5" t="s">
-        <v>904</v>
+        <v>939</v>
+      </c>
+      <c r="S197" s="0" t="s">
+        <v>940</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>905</v>
+        <v>827</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>434</v>
+        <v>941</v>
       </c>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
       <c r="E198" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F198" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H198" s="0" t="s">
         <v>24</v>
       </c>
@@ -13310,34 +13598,40 @@
       <c r="J198" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K198" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L198" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M198" s="5" t="s">
-        <v>906</v>
+        <v>942</v>
       </c>
       <c r="N198" s="5" t="s">
-        <v>907</v>
+        <v>943</v>
+      </c>
+      <c r="O198" s="0" t="s">
+        <v>944</v>
       </c>
       <c r="Q198" s="5" t="s">
-        <v>908</v>
+        <v>945</v>
+      </c>
+      <c r="S198" s="0" t="s">
+        <v>946</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>905</v>
+        <v>827</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>439</v>
+        <v>947</v>
       </c>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
       <c r="E199" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F199" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H199" s="0" t="s">
         <v>24</v>
       </c>
@@ -13347,34 +13641,40 @@
       <c r="J199" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K199" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L199" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M199" s="5" t="s">
-        <v>909</v>
+        <v>948</v>
       </c>
       <c r="N199" s="5" t="s">
-        <v>910</v>
+        <v>949</v>
+      </c>
+      <c r="O199" s="0" t="s">
+        <v>950</v>
       </c>
       <c r="Q199" s="5" t="s">
-        <v>911</v>
+        <v>951</v>
+      </c>
+      <c r="S199" s="0" t="s">
+        <v>952</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>905</v>
+        <v>827</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>428</v>
+        <v>953</v>
       </c>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
       <c r="E200" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F200" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H200" s="0" t="s">
         <v>24</v>
       </c>
@@ -13384,29 +13684,34 @@
       <c r="J200" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K200" s="0" t="s">
-        <v>828</v>
-      </c>
       <c r="L200" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M200" s="5" t="s">
-        <v>912</v>
+        <v>954</v>
       </c>
       <c r="N200" s="5" t="s">
-        <v>913</v>
+        <v>955</v>
+      </c>
+      <c r="O200" s="0" t="s">
+        <v>956</v>
       </c>
       <c r="Q200" s="5" t="s">
-        <v>914</v>
+        <v>957</v>
+      </c>
+      <c r="S200" s="0" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>915</v>
+        <v>959</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>315</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
       <c r="E201" s="0" t="s">
         <v>24</v>
       </c>
@@ -13414,49 +13719,42 @@
         <v>24</v>
       </c>
       <c r="H201" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I201" s="0" t="s">
         <v>26</v>
       </c>
       <c r="J201" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K201" s="0" t="s">
-        <v>916</v>
+        <v>25</v>
       </c>
       <c r="L201" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M201" s="5" t="s">
-        <v>917</v>
+        <v>960</v>
       </c>
       <c r="N201" s="5" t="s">
-        <v>918</v>
+        <v>961</v>
       </c>
       <c r="O201" s="0" t="s">
-        <v>919</v>
-      </c>
-      <c r="P201" s="5" t="s">
-        <v>920</v>
+        <v>962</v>
       </c>
       <c r="Q201" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="R201" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="S201" s="5" t="s">
-        <v>921</v>
+        <v>963</v>
+      </c>
+      <c r="S201" s="0" t="s">
+        <v>964</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>915</v>
+        <v>959</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>107</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="C202" s="5"/>
+      <c r="D202" s="5"/>
       <c r="E202" s="0" t="s">
         <v>24</v>
       </c>
@@ -13464,7 +13762,7 @@
         <v>24</v>
       </c>
       <c r="H202" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I202" s="0" t="s">
         <v>30</v>
@@ -13472,41 +13770,39 @@
       <c r="J202" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K202" s="0" t="s">
-        <v>916</v>
-      </c>
       <c r="L202" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M202" s="5" t="s">
-        <v>922</v>
-      </c>
-      <c r="N202" s="5"/>
+        <v>965</v>
+      </c>
+      <c r="N202" s="5" t="s">
+        <v>966</v>
+      </c>
       <c r="O202" s="0" t="s">
-        <v>923</v>
-      </c>
-      <c r="P202" s="5" t="s">
-        <v>920</v>
+        <v>967</v>
       </c>
       <c r="Q202" s="5" t="s">
-        <v>924</v>
-      </c>
-      <c r="R202" s="5" t="n">
-        <v>2</v>
+        <v>968</v>
+      </c>
+      <c r="S202" s="0" t="s">
+        <v>969</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>915</v>
+        <v>959</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>659</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="C203" s="5"/>
+      <c r="D203" s="5"/>
       <c r="E203" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F203" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H203" s="0" t="s">
         <v>24</v>
@@ -13517,35 +13813,34 @@
       <c r="J203" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K203" s="0" t="s">
-        <v>916</v>
-      </c>
       <c r="L203" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M203" s="5" t="s">
-        <v>925</v>
+        <v>970</v>
       </c>
       <c r="N203" s="5" t="s">
-        <v>926</v>
-      </c>
-      <c r="P203" s="5" t="s">
-        <v>920</v>
+        <v>971</v>
+      </c>
+      <c r="O203" s="0" t="s">
+        <v>972</v>
       </c>
       <c r="Q203" s="5" t="s">
-        <v>927</v>
-      </c>
-      <c r="R203" s="5" t="n">
-        <v>2</v>
+        <v>973</v>
+      </c>
+      <c r="S203" s="0" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>915</v>
+        <v>959</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>150</v>
-      </c>
+        <v>975</v>
+      </c>
+      <c r="C204" s="5"/>
+      <c r="D204" s="5"/>
       <c r="E204" s="0" t="s">
         <v>24</v>
       </c>
@@ -13561,41 +13856,34 @@
       <c r="J204" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K204" s="0" t="s">
-        <v>916</v>
-      </c>
       <c r="L204" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M204" s="5" t="s">
-        <v>928</v>
+        <v>976</v>
       </c>
       <c r="N204" s="5" t="s">
-        <v>929</v>
+        <v>977</v>
       </c>
       <c r="O204" s="0" t="s">
-        <v>930</v>
-      </c>
-      <c r="P204" s="5" t="s">
-        <v>920</v>
+        <v>978</v>
       </c>
       <c r="Q204" s="5" t="s">
-        <v>931</v>
-      </c>
-      <c r="R204" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="S204" s="5" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>979</v>
+      </c>
+      <c r="S204" s="0" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>915</v>
+        <v>959</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>319</v>
-      </c>
+        <v>468</v>
+      </c>
+      <c r="C205" s="5"/>
+      <c r="D205" s="5"/>
       <c r="E205" s="0" t="s">
         <v>24</v>
       </c>
@@ -13611,37 +13899,31 @@
       <c r="J205" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K205" s="0" t="s">
-        <v>916</v>
-      </c>
       <c r="L205" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M205" s="5" t="s">
-        <v>933</v>
-      </c>
-      <c r="N205" s="5" t="s">
-        <v>934</v>
-      </c>
-      <c r="P205" s="5" t="s">
-        <v>920</v>
+        <v>981</v>
+      </c>
+      <c r="N205" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="O205" s="0" t="s">
+        <v>983</v>
       </c>
       <c r="Q205" s="5" t="s">
-        <v>657</v>
-      </c>
-      <c r="R205" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="S205" s="5" t="s">
-        <v>935</v>
+        <v>983</v>
+      </c>
+      <c r="S205" s="9" t="s">
+        <v>984</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>915</v>
+        <v>985</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>936</v>
+        <v>315</v>
       </c>
       <c r="E206" s="0" t="s">
         <v>24</v>
@@ -13653,42 +13935,45 @@
         <v>24</v>
       </c>
       <c r="I206" s="0" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="J206" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K206" s="0" t="s">
-        <v>916</v>
+        <v>986</v>
       </c>
       <c r="L206" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M206" s="5" t="s">
-        <v>937</v>
+        <v>987</v>
       </c>
       <c r="N206" s="5" t="s">
-        <v>938</v>
+        <v>988</v>
+      </c>
+      <c r="O206" s="0" t="s">
+        <v>989</v>
       </c>
       <c r="P206" s="5" t="s">
-        <v>920</v>
+        <v>990</v>
       </c>
       <c r="Q206" s="5" t="s">
-        <v>939</v>
+        <v>508</v>
       </c>
       <c r="R206" s="5" t="n">
         <v>1</v>
       </c>
       <c r="S206" s="5" t="s">
-        <v>940</v>
+        <v>991</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>915</v>
+        <v>985</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>619</v>
+        <v>107</v>
       </c>
       <c r="E207" s="0" t="s">
         <v>24</v>
@@ -13697,174 +13982,184 @@
         <v>24</v>
       </c>
       <c r="H207" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I207" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="J207" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K207" s="0" t="s">
-        <v>916</v>
+        <v>986</v>
       </c>
       <c r="L207" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M207" s="5" t="s">
-        <v>941</v>
-      </c>
-      <c r="N207" s="5" t="s">
-        <v>942</v>
+        <v>992</v>
+      </c>
+      <c r="N207" s="5"/>
+      <c r="O207" s="0" t="s">
+        <v>993</v>
       </c>
       <c r="P207" s="5" t="s">
-        <v>920</v>
+        <v>990</v>
       </c>
       <c r="Q207" s="5" t="s">
-        <v>943</v>
+        <v>831</v>
       </c>
       <c r="R207" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="S207" s="5"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>944</v>
+        <v>985</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>434</v>
+        <v>659</v>
       </c>
       <c r="E208" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F208" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="H208" s="0" t="s">
         <v>24</v>
       </c>
       <c r="I208" s="0" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="J208" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K208" s="0" t="s">
-        <v>916</v>
+        <v>986</v>
       </c>
       <c r="L208" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M208" s="5" t="s">
-        <v>945</v>
+        <v>994</v>
       </c>
       <c r="N208" s="5" t="s">
-        <v>946</v>
+        <v>995</v>
       </c>
       <c r="P208" s="5" t="s">
-        <v>348</v>
+        <v>990</v>
       </c>
       <c r="Q208" s="5" t="s">
-        <v>947</v>
+        <v>996</v>
       </c>
       <c r="R208" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="S208" s="5" t="s">
-        <v>948</v>
+        <v>2</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>944</v>
+        <v>985</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>439</v>
+        <v>150</v>
       </c>
       <c r="E209" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F209" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="H209" s="0" t="s">
         <v>24</v>
       </c>
       <c r="I209" s="0" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="J209" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K209" s="0" t="s">
-        <v>916</v>
+        <v>986</v>
       </c>
       <c r="L209" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M209" s="5" t="s">
-        <v>949</v>
+        <v>997</v>
       </c>
       <c r="N209" s="5" t="s">
-        <v>950</v>
+        <v>998</v>
+      </c>
+      <c r="O209" s="0" t="s">
+        <v>999</v>
       </c>
       <c r="P209" s="5" t="s">
-        <v>348</v>
+        <v>990</v>
       </c>
       <c r="Q209" s="5" t="s">
-        <v>951</v>
+        <v>1000</v>
       </c>
       <c r="R209" s="5" t="n">
         <v>1</v>
       </c>
       <c r="S209" s="5" t="s">
-        <v>952</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>944</v>
+        <v>985</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>428</v>
+        <v>319</v>
       </c>
       <c r="E210" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="F210" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="H210" s="0" t="s">
         <v>24</v>
       </c>
       <c r="I210" s="0" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="J210" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K210" s="0" t="s">
-        <v>916</v>
+        <v>986</v>
       </c>
       <c r="L210" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M210" s="5" t="s">
-        <v>953</v>
+        <v>1002</v>
       </c>
       <c r="N210" s="5" t="s">
-        <v>954</v>
+        <v>1003</v>
       </c>
       <c r="P210" s="5" t="s">
-        <v>348</v>
+        <v>990</v>
       </c>
       <c r="Q210" s="5" t="s">
-        <v>955</v>
+        <v>657</v>
       </c>
       <c r="R210" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="S210" s="5"/>
+      <c r="S210" s="5" t="s">
+        <v>1004</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="5"/>
+      <c r="A211" s="0" t="s">
+        <v>985</v>
+      </c>
       <c r="B211" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D211" s="0" t="s">
-        <v>956</v>
+        <v>1005</v>
       </c>
       <c r="E211" s="0" t="s">
         <v>24</v>
@@ -13876,59 +14171,42 @@
         <v>24</v>
       </c>
       <c r="I211" s="0" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="J211" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K211" s="0" t="s">
-        <v>307</v>
+        <v>986</v>
       </c>
       <c r="L211" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M211" s="0" t="s">
-        <v>957</v>
-      </c>
-      <c r="O211" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="P211" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q211" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="R211" s="0" t="n">
+      <c r="M211" s="5" t="s">
+        <v>1006</v>
+      </c>
+      <c r="N211" s="5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P211" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="Q211" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="R211" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S211" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="T211" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="AA211" s="3"/>
-      <c r="AB211" s="3"/>
-      <c r="AC211" s="3"/>
-      <c r="AD211" s="3"/>
-      <c r="AE211" s="3"/>
-      <c r="AF211" s="3"/>
-      <c r="AG211" s="3"/>
-      <c r="AH211" s="3"/>
-      <c r="AI211" s="3"/>
-      <c r="AJ211" s="3"/>
-      <c r="AK211" s="3"/>
-      <c r="AL211" s="3"/>
+      <c r="S211" s="5" t="s">
+        <v>1009</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="5"/>
+      <c r="A212" s="0" t="s">
+        <v>985</v>
+      </c>
       <c r="B212" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="C212" s="5"/>
-      <c r="D212" s="0" t="s">
-        <v>956</v>
+        <v>619</v>
       </c>
       <c r="E212" s="0" t="s">
         <v>24</v>
@@ -13940,369 +14218,434 @@
         <v>24</v>
       </c>
       <c r="I212" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J212" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K212" s="0" t="s">
-        <v>307</v>
+        <v>986</v>
       </c>
       <c r="L212" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M212" s="0" t="s">
-        <v>958</v>
-      </c>
-      <c r="O212" s="0" t="s">
-        <v>520</v>
-      </c>
-      <c r="P212" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q212" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="R212" s="0" t="n">
+      <c r="M212" s="5" t="s">
+        <v>1010</v>
+      </c>
+      <c r="N212" s="5" t="s">
+        <v>1011</v>
+      </c>
+      <c r="P212" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="Q212" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R212" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S212" s="5"/>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="E213" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H213" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I213" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J213" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K213" s="0" t="s">
+        <v>986</v>
+      </c>
+      <c r="L213" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M213" s="5" t="s">
+        <v>1014</v>
+      </c>
+      <c r="N213" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="P213" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q213" s="5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="R213" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="S212" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="T212" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="AA212" s="3"/>
-      <c r="AB212" s="3"/>
-      <c r="AC212" s="3"/>
-      <c r="AD212" s="3"/>
-      <c r="AE212" s="3"/>
-      <c r="AF212" s="3"/>
-      <c r="AG212" s="3"/>
-      <c r="AH212" s="3"/>
-      <c r="AI212" s="3"/>
-      <c r="AJ212" s="3"/>
-      <c r="AK212" s="3"/>
-      <c r="AL212" s="3"/>
-    </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="5"/>
-      <c r="B213" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D213" s="0" t="s">
-        <v>956</v>
-      </c>
-      <c r="E213" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F213" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H213" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I213" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J213" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K213" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="L213" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M213" s="0" t="s">
-        <v>959</v>
-      </c>
-      <c r="O213" s="0" t="s">
-        <v>924</v>
-      </c>
-      <c r="P213" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q213" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="R213" s="0" t="n">
+      <c r="S213" s="5" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="E214" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H214" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I214" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J214" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K214" s="0" t="s">
+        <v>986</v>
+      </c>
+      <c r="L214" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M214" s="5" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N214" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P214" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q214" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="R214" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="AA213" s="3"/>
-      <c r="AB213" s="3"/>
-      <c r="AC213" s="3"/>
-      <c r="AD213" s="3"/>
-      <c r="AE213" s="3"/>
-      <c r="AF213" s="3"/>
-      <c r="AG213" s="3"/>
-      <c r="AH213" s="3"/>
-      <c r="AI213" s="3"/>
-      <c r="AJ213" s="3"/>
-      <c r="AK213" s="3"/>
-      <c r="AL213" s="3"/>
-    </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="D214" s="0" t="s">
-        <v>956</v>
-      </c>
-      <c r="E214" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F214" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H214" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I214" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="J214" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K214" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="L214" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M214" s="0" t="s">
-        <v>960</v>
-      </c>
-      <c r="O214" s="0" t="s">
-        <v>961</v>
-      </c>
-      <c r="P214" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q214" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="R214" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S214" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="T214" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="U214" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="V214" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="AA214" s="3"/>
-      <c r="AB214" s="3"/>
-      <c r="AC214" s="3"/>
-      <c r="AD214" s="3"/>
-      <c r="AE214" s="3"/>
-      <c r="AF214" s="3"/>
-      <c r="AG214" s="3"/>
-      <c r="AH214" s="3"/>
-      <c r="AI214" s="3"/>
-      <c r="AJ214" s="3"/>
-      <c r="AK214" s="3"/>
-      <c r="AL214" s="3"/>
+      <c r="S214" s="5" t="s">
+        <v>1021</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>962</v>
+        <v>1013</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="E215" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F215" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H215" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I215" s="0" t="n">
-        <v>0</v>
+        <v>428</v>
+      </c>
+      <c r="E215" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H215" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I215" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="J215" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="K215" s="0" t="s">
+        <v>986</v>
       </c>
       <c r="L215" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M215" s="0" t="s">
-        <v>963</v>
-      </c>
-      <c r="O215" s="0" t="s">
-        <v>964</v>
-      </c>
-      <c r="Q215" s="0" t="s">
-        <v>964</v>
-      </c>
+      <c r="M215" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="N215" s="5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P215" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q215" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="R215" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="S215" s="5"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
-        <v>962</v>
-      </c>
+      <c r="A216" s="5"/>
       <c r="B216" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="E216" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F216" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H216" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I216" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D216" s="0" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E216" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F216" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H216" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I216" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J216" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K216" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="L216" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M216" s="0" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O216" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="P216" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q216" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="R216" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J216" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L216" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M216" s="0" t="s">
-        <v>965</v>
-      </c>
-      <c r="O216" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q216" s="0" t="s">
-        <v>219</v>
-      </c>
+      <c r="S216" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="T216" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="AA216" s="3"/>
+      <c r="AB216" s="3"/>
+      <c r="AC216" s="3"/>
+      <c r="AD216" s="3"/>
+      <c r="AE216" s="3"/>
+      <c r="AF216" s="3"/>
+      <c r="AG216" s="3"/>
+      <c r="AH216" s="3"/>
+      <c r="AI216" s="3"/>
+      <c r="AJ216" s="3"/>
+      <c r="AK216" s="3"/>
+      <c r="AL216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
-        <v>962</v>
-      </c>
+      <c r="A217" s="5"/>
       <c r="B217" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="E217" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F217" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H217" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I217" s="0" t="n">
-        <v>2</v>
+        <v>319</v>
+      </c>
+      <c r="C217" s="5"/>
+      <c r="D217" s="0" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E217" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F217" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H217" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I217" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="J217" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="K217" s="0" t="s">
+        <v>307</v>
       </c>
       <c r="L217" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M217" s="0" t="s">
-        <v>966</v>
+        <v>1027</v>
       </c>
       <c r="O217" s="0" t="s">
-        <v>222</v>
+        <v>520</v>
+      </c>
+      <c r="P217" s="0" t="s">
+        <v>311</v>
       </c>
       <c r="Q217" s="0" t="s">
-        <v>222</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="R217" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S217" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="T217" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="AA217" s="3"/>
+      <c r="AB217" s="3"/>
+      <c r="AC217" s="3"/>
+      <c r="AD217" s="3"/>
+      <c r="AE217" s="3"/>
+      <c r="AF217" s="3"/>
+      <c r="AG217" s="3"/>
+      <c r="AH217" s="3"/>
+      <c r="AI217" s="3"/>
+      <c r="AJ217" s="3"/>
+      <c r="AK217" s="3"/>
+      <c r="AL217" s="3"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
-        <v>962</v>
-      </c>
+      <c r="A218" s="5"/>
       <c r="B218" s="0" t="s">
-        <v>967</v>
-      </c>
-      <c r="E218" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F218" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H218" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I218" s="0" t="n">
-        <v>4</v>
+        <v>107</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E218" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F218" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H218" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I218" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="J218" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="K218" s="0" t="s">
+        <v>307</v>
       </c>
       <c r="L218" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M218" s="0" t="s">
-        <v>968</v>
+        <v>1028</v>
       </c>
       <c r="O218" s="0" t="s">
-        <v>969</v>
+        <v>831</v>
+      </c>
+      <c r="P218" s="0" t="s">
+        <v>311</v>
       </c>
       <c r="Q218" s="0" t="s">
-        <v>970</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="R218" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA218" s="3"/>
+      <c r="AB218" s="3"/>
+      <c r="AC218" s="3"/>
+      <c r="AD218" s="3"/>
+      <c r="AE218" s="3"/>
+      <c r="AF218" s="3"/>
+      <c r="AG218" s="3"/>
+      <c r="AH218" s="3"/>
+      <c r="AI218" s="3"/>
+      <c r="AJ218" s="3"/>
+      <c r="AK218" s="3"/>
+      <c r="AL218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
-        <v>962</v>
-      </c>
       <c r="B219" s="0" t="s">
-        <v>971</v>
-      </c>
-      <c r="E219" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F219" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H219" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I219" s="0" t="n">
-        <v>3</v>
+        <v>352</v>
+      </c>
+      <c r="D219" s="0" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E219" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F219" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H219" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I219" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="J219" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="K219" s="0" t="s">
+        <v>307</v>
       </c>
       <c r="L219" s="0" t="s">
         <v>24</v>
       </c>
       <c r="M219" s="0" t="s">
-        <v>972</v>
+        <v>1029</v>
       </c>
       <c r="O219" s="0" t="s">
-        <v>973</v>
+        <v>1030</v>
+      </c>
+      <c r="P219" s="0" t="s">
+        <v>311</v>
       </c>
       <c r="Q219" s="0" t="s">
-        <v>974</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="R219" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S219" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="T219" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="U219" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="V219" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA219" s="3"/>
+      <c r="AB219" s="3"/>
+      <c r="AC219" s="3"/>
+      <c r="AD219" s="3"/>
+      <c r="AE219" s="3"/>
+      <c r="AF219" s="3"/>
+      <c r="AG219" s="3"/>
+      <c r="AH219" s="3"/>
+      <c r="AI219" s="3"/>
+      <c r="AJ219" s="3"/>
+      <c r="AK219" s="3"/>
+      <c r="AL219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>962</v>
+        <v>1031</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>975</v>
+        <v>215</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F220" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H220" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I220" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J220" s="0" t="s">
         <v>25</v>
@@ -14311,33 +14654,33 @@
         <v>24</v>
       </c>
       <c r="M220" s="0" t="s">
-        <v>976</v>
+        <v>1032</v>
       </c>
       <c r="O220" s="0" t="s">
-        <v>977</v>
+        <v>1033</v>
       </c>
       <c r="Q220" s="0" t="s">
-        <v>978</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>1031</v>
+      </c>
       <c r="B221" s="0" t="s">
-        <v>979</v>
-      </c>
-      <c r="D221" s="0" t="s">
-        <v>962</v>
+        <v>221</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F221" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H221" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I221" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J221" s="0" t="s">
         <v>25</v>
@@ -14346,33 +14689,33 @@
         <v>24</v>
       </c>
       <c r="M221" s="0" t="s">
-        <v>980</v>
+        <v>1034</v>
       </c>
       <c r="O221" s="0" t="s">
-        <v>981</v>
+        <v>219</v>
       </c>
       <c r="Q221" s="0" t="s">
-        <v>982</v>
+        <v>219</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>983</v>
-      </c>
-      <c r="B222" s="5" t="s">
-        <v>224</v>
+        <v>1031</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>218</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F222" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H222" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I222" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J222" s="0" t="s">
         <v>25</v>
@@ -14381,33 +14724,33 @@
         <v>24</v>
       </c>
       <c r="M222" s="0" t="s">
-        <v>984</v>
+        <v>1035</v>
       </c>
       <c r="O222" s="0" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="Q222" s="0" t="s">
-        <v>985</v>
+        <v>222</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>983</v>
-      </c>
-      <c r="B223" s="5" t="s">
-        <v>227</v>
+        <v>1031</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>1036</v>
       </c>
       <c r="E223" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F223" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H223" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I223" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J223" s="0" t="s">
         <v>25</v>
@@ -14416,48 +14759,223 @@
         <v>24</v>
       </c>
       <c r="M223" s="0" t="s">
-        <v>986</v>
+        <v>1037</v>
       </c>
       <c r="O223" s="0" t="s">
-        <v>228</v>
+        <v>1038</v>
       </c>
       <c r="Q223" s="0" t="s">
-        <v>228</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>983</v>
+        <v>1031</v>
       </c>
       <c r="B224" s="0" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E224" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F224" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H224" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I224" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J224" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L224" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M224" s="0" t="s">
+        <v>1041</v>
+      </c>
+      <c r="O224" s="0" t="s">
+        <v>1042</v>
+      </c>
+      <c r="Q224" s="0" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E225" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F225" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H225" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I225" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J225" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L225" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M225" s="0" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O225" s="0" t="s">
+        <v>1046</v>
+      </c>
+      <c r="Q225" s="0" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B226" s="0" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D226" s="0" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E226" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F226" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H226" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I226" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J226" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L226" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M226" s="0" t="s">
+        <v>1049</v>
+      </c>
+      <c r="O226" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="Q226" s="0" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E227" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F227" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H227" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I227" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J227" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L227" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M227" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="O227" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q227" s="0" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E228" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F228" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H228" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I228" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J228" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L228" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M228" s="0" t="s">
+        <v>1055</v>
+      </c>
+      <c r="O228" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q228" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B229" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="E224" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F224" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H224" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I224" s="0" t="n">
+      <c r="E229" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F229" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H229" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I229" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="J224" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L224" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M224" s="0" t="s">
-        <v>987</v>
-      </c>
-      <c r="O224" s="0" t="s">
-        <v>988</v>
-      </c>
-      <c r="Q224" s="0" t="s">
-        <v>988</v>
+      <c r="J229" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L229" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M229" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O229" s="0" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Q229" s="0" t="s">
+        <v>1057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set new unassigned fields as "not lincs field"
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -3364,11 +3364,11 @@
   <dimension ref="A1:AR229"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J178" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F180" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A178" activeCellId="0" sqref="A178"/>
-      <selection pane="bottomRight" activeCell="O200" activeCellId="0" sqref="O200"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A180" activeCellId="0" sqref="A180"/>
+      <selection pane="bottomRight" activeCell="H182" activeCellId="0" sqref="H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -12865,7 +12865,7 @@
         <v>24</v>
       </c>
       <c r="H181" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I181" s="0" t="s">
         <v>37</v>
@@ -12951,7 +12951,7 @@
         <v>24</v>
       </c>
       <c r="H183" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I183" s="0" t="s">
         <v>45</v>
@@ -13076,7 +13076,7 @@
         <v>25</v>
       </c>
       <c r="H186" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I186" s="0" t="s">
         <v>56</v>
@@ -13117,7 +13117,7 @@
         <v>25</v>
       </c>
       <c r="H187" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I187" s="0" t="s">
         <v>59</v>
@@ -13160,7 +13160,7 @@
         <v>25</v>
       </c>
       <c r="H188" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I188" s="0" t="s">
         <v>63</v>
@@ -13246,7 +13246,7 @@
         <v>25</v>
       </c>
       <c r="H190" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I190" s="0" t="s">
         <v>71</v>
@@ -13418,7 +13418,7 @@
         <v>25</v>
       </c>
       <c r="H194" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I194" s="0" t="s">
         <v>85</v>
@@ -13633,7 +13633,7 @@
         <v>25</v>
       </c>
       <c r="H199" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I199" s="0" t="s">
         <v>103</v>

</xml_diff>